<commit_message>
clean up and minor bug fixes in forms
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-maturity sorting.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-maturity sorting.xlsx
@@ -141,7 +141,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -200,6 +200,7 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +486,7 @@
   <dimension ref="A1:H890"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,11 +529,7 @@
       <c r="F2" s="8"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="20"/>
-    </row>
+    <row r="3" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F4" s="8"/>
     </row>

</xml_diff>